<commit_message>
Update BOM, add TODO
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="GIRA_ESP8266_Jalousiesteuerung" localSheetId="0">Tabelle1!$A$1:$F$14</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -186,18 +186,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,10 +214,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -221,9 +227,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,7 +543,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +583,7 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -593,7 +603,7 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -613,7 +623,7 @@
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -633,7 +643,7 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -693,7 +703,7 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -713,6 +723,7 @@
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
@@ -790,6 +801,7 @@
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
@@ -807,7 +819,7 @@
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="1" t="s">

</xml_diff>